<commit_message>
add get req archive
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -609,22 +609,22 @@
         <v>12</v>
       </c>
       <c r="D4" s="3">
-        <v>645</v>
+        <v>536</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="3">
-        <v>0.766</v>
+        <v>567</v>
       </c>
       <c r="G4" s="3">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="H4" s="3">
-        <v>53.4</v>
+        <v>2</v>
       </c>
       <c r="I4" s="3">
-        <v>0.34</v>
+        <v>6</v>
       </c>
       <c r="J4" s="4">
         <f>ROUND(1.0*D4*F4*G4, 2)</f>
@@ -652,22 +652,22 @@
         <v>14</v>
       </c>
       <c r="D5" s="3">
-        <v>131</v>
+        <v>534</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="3">
-        <v>0.766</v>
+        <v>567</v>
       </c>
       <c r="G5" s="3">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="H5" s="3">
-        <v>53.4</v>
+        <v>2</v>
       </c>
       <c r="I5" s="3">
-        <v>0.34</v>
+        <v>6</v>
       </c>
       <c r="J5" s="4">
         <f>ROUND(1.0*D5*F5*G5, 2)</f>
@@ -695,22 +695,22 @@
         <v>15</v>
       </c>
       <c r="D6" s="3">
-        <v>312</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="3">
-        <v>0.766</v>
+        <v>567</v>
       </c>
       <c r="G6" s="3">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="H6" s="3">
-        <v>53.4</v>
+        <v>2</v>
       </c>
       <c r="I6" s="3">
-        <v>0.34</v>
+        <v>6</v>
       </c>
       <c r="J6" s="4">
         <f>ROUND(1.0*D6*F6*G6, 2)</f>
@@ -781,25 +781,25 @@
         <v>12</v>
       </c>
       <c r="D12" s="3">
-        <v>645</v>
+        <v>536</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="3">
-        <v>0.766</v>
+        <v>567</v>
       </c>
       <c r="G12" s="3">
-        <v>312</v>
+        <v>533</v>
       </c>
       <c r="H12" s="3">
-        <v>321</v>
+        <v>75</v>
       </c>
       <c r="I12" s="3">
-        <v>321</v>
+        <v>567</v>
       </c>
       <c r="J12" s="3">
-        <v>312</v>
+        <v>43</v>
       </c>
       <c r="K12" s="7">
         <f>ROUND(1.0*D12*F12*G12*H12, 2)</f>
@@ -823,25 +823,25 @@
         <v>14</v>
       </c>
       <c r="D13" s="3">
-        <v>131</v>
+        <v>534</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="3">
-        <v>0.766</v>
+        <v>567</v>
       </c>
       <c r="G13" s="3">
-        <v>312</v>
+        <v>533</v>
       </c>
       <c r="H13" s="3">
-        <v>321</v>
+        <v>75</v>
       </c>
       <c r="I13" s="3">
-        <v>321</v>
+        <v>567</v>
       </c>
       <c r="J13" s="3">
-        <v>312</v>
+        <v>43</v>
       </c>
       <c r="K13" s="7">
         <f>ROUND(1.0*D13*F13*G13*H13, 2)</f>
@@ -865,25 +865,25 @@
         <v>15</v>
       </c>
       <c r="D14" s="3">
-        <v>312</v>
+        <v>53</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="3">
-        <v>0.766</v>
+        <v>567</v>
       </c>
       <c r="G14" s="3">
-        <v>312</v>
+        <v>533</v>
       </c>
       <c r="H14" s="3">
-        <v>321</v>
+        <v>75</v>
       </c>
       <c r="I14" s="3">
-        <v>321</v>
+        <v>567</v>
       </c>
       <c r="J14" s="3">
-        <v>312</v>
+        <v>43</v>
       </c>
       <c r="K14" s="7">
         <f>ROUND(1.0*D14*F14*G14*H14, 2)</f>
@@ -959,13 +959,13 @@
         <v>12</v>
       </c>
       <c r="C20" s="3">
-        <v>645</v>
+        <v>1534</v>
       </c>
       <c r="D20" s="3">
-        <v>645</v>
+        <v>536</v>
       </c>
       <c r="E20" s="3">
-        <v>645</v>
+        <v>345</v>
       </c>
       <c r="F20" s="5">
         <f>ROUND(D20*C20/E20, 2)</f>
@@ -975,13 +975,13 @@
         <v>14</v>
       </c>
       <c r="I20" s="3">
-        <v>231</v>
+        <v>45</v>
       </c>
       <c r="J20" s="3">
-        <v>131</v>
+        <v>534</v>
       </c>
       <c r="K20" s="3">
-        <v>321</v>
+        <v>645</v>
       </c>
       <c r="L20" s="5">
         <f>ROUND(J20/K20, 2)</f>
@@ -991,13 +991,13 @@
         <v>15</v>
       </c>
       <c r="O20" s="3">
+        <v>745</v>
+      </c>
+      <c r="P20" s="3">
+        <v>53</v>
+      </c>
+      <c r="Q20" s="3">
         <v>64</v>
-      </c>
-      <c r="P20" s="3">
-        <v>312</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>45</v>
       </c>
       <c r="R20" s="5">
         <f>ROUND(P20/Q20, 2)</f>

</xml_diff>